<commit_message>
Préparer la publication 1.4.1506.0.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,23 +7,24 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId1"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId2"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId3"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId4"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId5"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId6"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId7"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId9"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId10"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId1"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId2"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId3"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId4"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId5"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId6"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId7"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId8"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId10"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="118">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -365,6 +366,18 @@
   </si>
   <si>
     <t>Importations, mails</t>
+  </si>
+  <si>
+    <t>Corrections et travaux divers</t>
+  </si>
+  <si>
+    <t>Gestion de projet</t>
+  </si>
+  <si>
+    <t>Facturé le 02.02.2015</t>
+  </si>
+  <si>
+    <t>Correctifs, investigations + Clarens</t>
   </si>
 </sst>
 </file>
@@ -775,10 +788,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,17 +841,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42007</v>
+        <v>42036</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
+        <f t="shared" ref="G4:G12" si="0">D4*F4</f>
         <v>0</v>
       </c>
     </row>
@@ -847,14 +860,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42012</v>
+        <v>42037</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>5.5555555555555552E-2</v>
+        <v>115</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
@@ -866,15 +878,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>42014</v>
+        <v>42037</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>9.375E-2</v>
+      </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -884,19 +895,8 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>42028</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="2"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -906,29 +906,18 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>42034</v>
-      </c>
-      <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="2">
-        <v>4.5138888888888888E-2</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>4.5138888888888888E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="1"/>
       <c r="D9" s="2"/>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -939,7 +928,7 @@
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="1"/>
       <c r="D10" s="2"/>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
@@ -950,7 +939,7 @@
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="1"/>
       <c r="D11" s="2"/>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -975,7 +964,7 @@
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G13:G35" si="1">D13*F13</f>
         <v>0</v>
       </c>
     </row>
@@ -986,7 +975,7 @@
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -997,7 +986,7 @@
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1008,7 +997,7 @@
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" ref="G16:G29" si="1">D16*F16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1071,17 +1060,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>41982</v>
+        <v>42037</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D23" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G26" si="2">D23*F23</f>
+        <f t="shared" ref="G23:G30" si="2">D23*F23</f>
         <v>0</v>
       </c>
     </row>
@@ -1089,15 +1078,8 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1">
-        <v>41983</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
       <c r="F24" s="8"/>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
@@ -1108,15 +1090,8 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
-        <v>41984</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.25694444444444448</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
       <c r="F25" s="8"/>
       <c r="G25" s="2">
         <f t="shared" si="2"/>
@@ -1127,16 +1102,8 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <v>41988</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="F26" s="8"/>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="G26" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1146,18 +1113,11 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <v>41996</v>
-      </c>
-      <c r="C27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="F27" s="8"/>
       <c r="G27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1169,7 +1129,7 @@
       <c r="D28" s="2"/>
       <c r="F28" s="8"/>
       <c r="G28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1181,7 +1141,7 @@
       <c r="D29" s="2"/>
       <c r="F29" s="8"/>
       <c r="G29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1191,9 +1151,8 @@
       </c>
       <c r="B30" s="1"/>
       <c r="D30" s="2"/>
-      <c r="F30" s="8"/>
       <c r="G30" s="2">
-        <f t="shared" ref="G30:G35" si="3">D30*F30</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1204,7 +1163,7 @@
       <c r="B31" s="1"/>
       <c r="D31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1216,7 +1175,7 @@
       <c r="D32" s="2"/>
       <c r="F32" s="8"/>
       <c r="G32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1228,7 +1187,7 @@
       <c r="D33" s="2"/>
       <c r="F33" s="8"/>
       <c r="G33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1240,7 +1199,7 @@
       <c r="D34" s="2"/>
       <c r="F34" s="8"/>
       <c r="G34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1251,23 +1210,23 @@
       <c r="B35" s="1"/>
       <c r="D35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>1.1631944444444444</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0.1875</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
         <f>SUM(G4:G37)</f>
-        <v>4.5138888888888888E-2</v>
+        <v>0</v>
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="13">
@@ -1282,11 +1241,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>1.1180555555555556</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>26.833333333333332</v>
+        <v>6.5</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1298,7 +1257,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>4025</v>
+        <v>975</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1356,6 +1315,17 @@
         <v>3375</v>
       </c>
       <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F48" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1377,7 +1347,614 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42007</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42012</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42014</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42028</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42034</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" ref="G16:G29" si="1">D16*F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41982</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G26" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41983</v>
+      </c>
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41984</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41988</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41996</v>
+      </c>
+      <c r="C27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="2">
+        <f t="shared" ref="G30:G35" si="3">D30*F30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>1.1631944444444444</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.1180555555555556</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>26.833333333333332</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>4025</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2025,7 +2602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2643,7 +3220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3282,7 +3859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3944,7 +4521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4482,7 +5059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5048,7 +5625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5612,16 +6189,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: import RCH et mise à jour pour release.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId1"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId2"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId3"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId4"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId5"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId6"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId7"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId8"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId10"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId11"/>
+    <sheet name="2015.10-14" sheetId="12" r:id="rId1"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId2"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId3"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId4"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId5"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId6"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId7"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId8"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId9"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId11"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="123">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -378,6 +379,21 @@
   </si>
   <si>
     <t>Correctifs, investigations + Clarens</t>
+  </si>
+  <si>
+    <t>Divers</t>
+  </si>
+  <si>
+    <t>Exportation bonne nouvelle, maintenance</t>
+  </si>
+  <si>
+    <t>Divers TODO</t>
+  </si>
+  <si>
+    <t>MAT[CH]</t>
+  </si>
+  <si>
+    <t>Facturé le 03.03.2015</t>
   </si>
 </sst>
 </file>
@@ -790,8 +806,8 @@
   </sheetPr>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,17 +857,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42036</v>
+        <v>42065</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>3.4722222222222224E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G12" si="0">D4*F4</f>
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
         <v>0</v>
       </c>
     </row>
@@ -859,17 +875,10 @@
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>42037</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="2"/>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G5:G9" si="1">D5*F5</f>
         <v>0</v>
       </c>
     </row>
@@ -877,17 +886,10 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>42037</v>
-      </c>
-      <c r="C6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="2">
-        <v>9.375E-2</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -898,7 +900,7 @@
       <c r="B7" s="1"/>
       <c r="D7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -909,7 +911,7 @@
       <c r="B8" s="1"/>
       <c r="D8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -920,7 +922,7 @@
       <c r="B9" s="1"/>
       <c r="D9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -964,7 +966,7 @@
       <c r="B13" s="1"/>
       <c r="D13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" ref="G13:G35" si="1">D13*F13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -975,7 +977,7 @@
       <c r="B14" s="1"/>
       <c r="D14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -986,7 +988,7 @@
       <c r="B15" s="1"/>
       <c r="D15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -997,7 +999,7 @@
       <c r="B16" s="1"/>
       <c r="D16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1008,7 +1010,7 @@
       <c r="B17" s="1"/>
       <c r="D17" s="2"/>
       <c r="G17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1019,7 +1021,7 @@
       <c r="B18" s="1"/>
       <c r="D18" s="2"/>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1027,7 +1029,7 @@
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1035,7 +1037,7 @@
       <c r="B20" s="1"/>
       <c r="D20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1043,7 +1045,7 @@
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1051,7 +1053,7 @@
       <c r="B22" s="1"/>
       <c r="D22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1060,17 +1062,16 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>42037</v>
+        <v>42065</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D23" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F23" s="8"/>
+        <v>0.25</v>
+      </c>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G30" si="2">D23*F23</f>
+        <f t="shared" ref="G23:G34" si="2">D23*F23</f>
         <v>0</v>
       </c>
     </row>
@@ -1080,7 +1081,6 @@
       </c>
       <c r="B24" s="1"/>
       <c r="D24" s="2"/>
-      <c r="F24" s="8"/>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1092,7 +1092,6 @@
       </c>
       <c r="B25" s="1"/>
       <c r="D25" s="2"/>
-      <c r="F25" s="8"/>
       <c r="G25" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1115,7 +1114,6 @@
       </c>
       <c r="B27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="F27" s="8"/>
       <c r="G27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1127,7 +1125,6 @@
       </c>
       <c r="B28" s="1"/>
       <c r="D28" s="2"/>
-      <c r="F28" s="8"/>
       <c r="G28" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1139,7 +1136,6 @@
       </c>
       <c r="B29" s="1"/>
       <c r="D29" s="2"/>
-      <c r="F29" s="8"/>
       <c r="G29" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1163,7 +1159,7 @@
       <c r="B31" s="1"/>
       <c r="D31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1173,9 +1169,8 @@
       </c>
       <c r="B32" s="1"/>
       <c r="D32" s="2"/>
-      <c r="F32" s="8"/>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1185,9 +1180,8 @@
       </c>
       <c r="B33" s="1"/>
       <c r="D33" s="2"/>
-      <c r="F33" s="8"/>
       <c r="G33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1197,9 +1191,8 @@
       </c>
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
-      <c r="F34" s="8"/>
       <c r="G34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1210,18 +1203,18 @@
       <c r="B35" s="1"/>
       <c r="D35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.27083333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>3.4722222222222224E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1241,11 +1234,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.27083333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1257,7 +1250,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>975</v>
+        <v>900</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1337,13 +1330,567 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>41767</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f>D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41768</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G27" si="0">D5*F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41771</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41771</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41772</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41773</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41774</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41775</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41775</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41778</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41758</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41760</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2">
+        <f>I16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41761</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2">
+        <f>I17*F17</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41764</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="2">
+        <f>I18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41765</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41766</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41767</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41768</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2">
+        <f>I22*F22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41771</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41772</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41773</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41774</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41775</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="13">
+        <f>SUM(D4:D29)</f>
+        <v>2.3958333333333335</v>
+      </c>
+      <c r="E30" s="13">
+        <f>SUM(E4:E29)</f>
+        <v>0.33680555555555552</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="13">
+        <f>SUM(G4:G29)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="13">
+        <f>SUM(I4:I29)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="12">
+        <f>D30-G30</f>
+        <v>1.8958333333333335</v>
+      </c>
+      <c r="E32" s="10">
+        <f>INT(DAY(D32)*24+HOUR(D32))+MINUTE(D32)/60</f>
+        <v>45.5</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="10">
+        <f>E32*150</f>
+        <v>6825</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1359,7 +1906,691 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42036</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G12" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42037</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42037</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9.375E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42045</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42051</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42053</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" ref="G13:G35" si="1">D13*F13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42037</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G30" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42043</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42052</v>
+      </c>
+      <c r="C25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42053</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42054</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42058</v>
+      </c>
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42059</v>
+      </c>
+      <c r="C29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42060</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42060</v>
+      </c>
+      <c r="C31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42061</v>
+      </c>
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42061</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42062</v>
+      </c>
+      <c r="C34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.958333333333333</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.11805555555555555</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0.40625</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>2.552083333333333</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>61.25</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>9187.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="9">
+        <v>9178.5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1954,7 +3185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2602,7 +3833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3220,7 +4451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3859,7 +5090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4521,7 +5752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5059,7 +6290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5623,570 +6854,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>41767</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E4" s="7">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f>D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41768</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" ref="G5:G27" si="0">D5*F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41771</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41771</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41772</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.18055555555555555</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41773</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41774</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>41775</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41775</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>41778</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>41758</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1">
-        <v>41760</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="2">
-        <f>I16*F16</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1">
-        <v>41761</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="2">
-        <f>I17*F17</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>41764</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="2">
-        <f>I18*F18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1">
-        <v>41765</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.18055555555555555</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
-        <v>41766</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>41767</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>41768</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="2">
-        <f>I22*F22</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41771</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41772</v>
-      </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41773</v>
-      </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41774</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41775</v>
-      </c>
-      <c r="C27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="13">
-        <f>SUM(D4:D29)</f>
-        <v>2.3958333333333335</v>
-      </c>
-      <c r="E30" s="13">
-        <f>SUM(E4:E29)</f>
-        <v>0.33680555555555552</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="13">
-        <f>SUM(G4:G29)</f>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="13">
-        <f>SUM(I4:I29)</f>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="12">
-        <f>D30-G30</f>
-        <v>1.8958333333333335</v>
-      </c>
-      <c r="E32" s="10">
-        <f>INT(DAY(D32)*24+HOUR(D32))+MINUTE(D32)/60</f>
-        <v>45.5</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="10">
-        <f>E32*150</f>
-        <v>6825</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: export Bonne Nouvelle du 26.03.2015.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="129">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -400,6 +400,18 @@
   </si>
   <si>
     <t>E-mails, suivi du projet</t>
+  </si>
+  <si>
+    <t>Territoires, paroisses, etc.</t>
+  </si>
+  <si>
+    <t>Déploiement et maintenance</t>
+  </si>
+  <si>
+    <t>Étiquettes Avery</t>
+  </si>
+  <si>
+    <t>Bonne Nouvelle</t>
   </si>
 </sst>
 </file>
@@ -813,7 +825,7 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,8 +911,15 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="1">
+        <v>42077</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G6" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -910,8 +929,16 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>42077</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
       <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -921,8 +948,15 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="1">
+        <v>42081</v>
+      </c>
+      <c r="C8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -932,8 +966,16 @@
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1">
+        <v>42082</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
       <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1128,8 +1170,15 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="1">
+        <v>42067</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.125</v>
+      </c>
       <c r="G26" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1139,8 +1188,15 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="1">
+        <v>42067</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1150,8 +1206,15 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="1">
+        <v>42069</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G28" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1161,8 +1224,15 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="1">
+        <v>42072</v>
+      </c>
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="G29" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1172,8 +1242,15 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
+      <c r="B30" s="1">
+        <v>42073</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="G30" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1183,8 +1260,15 @@
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
+      <c r="B31" s="1">
+        <v>42075</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="G31" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1194,8 +1278,15 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="1">
+        <v>42076</v>
+      </c>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G32" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1205,8 +1296,15 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="1">
+        <v>42079</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G33" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1216,8 +1314,15 @@
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="1">
+        <v>42080</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="G34" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1227,8 +1332,15 @@
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
+      <c r="B35" s="1">
+        <v>42081</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.25</v>
+      </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1237,11 +1349,11 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.61805555555555558</v>
+        <v>2.5625000000000004</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>5.5555555555555552E-2</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1261,11 +1373,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.61805555555555558</v>
+        <v>2.5625000000000004</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>14.833333333333334</v>
+        <v>61.5</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1277,7 +1389,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>2225</v>
+        <v>9225</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Aider: mise à jour documents liés.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="131">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>Bonne Nouvelle</t>
+  </si>
+  <si>
+    <t>Divers, gestion de projet</t>
+  </si>
+  <si>
+    <t>Facturé le 29.03.2015</t>
   </si>
 </sst>
 </file>
@@ -822,10 +828,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,8 +991,15 @@
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="1">
+        <v>42092</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1349,7 +1362,7 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>2.5625000000000004</v>
+        <v>2.5729166666666674</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1373,11 +1386,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>2.5625000000000004</v>
+        <v>2.5729166666666674</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>61.5</v>
+        <v>61.75</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1389,29 +1402,18 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>9225</v>
+        <v>9262.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E44" s="9">
-        <v>7975.05</v>
+        <v>6900</v>
       </c>
       <c r="F44" t="s">
         <v>26</v>
@@ -1419,10 +1421,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E45" s="9">
-        <v>4762.5</v>
+        <v>7975.05</v>
       </c>
       <c r="F45" t="s">
         <v>26</v>
@@ -1430,10 +1432,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E46" s="9">
-        <v>5960</v>
+        <v>4762.5</v>
       </c>
       <c r="F46" t="s">
         <v>26</v>
@@ -1441,10 +1443,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E47" s="9">
-        <v>3375</v>
+        <v>5960</v>
       </c>
       <c r="F47" t="s">
         <v>26</v>
@@ -1452,12 +1454,34 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>116</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E49" s="9">
         <v>4025</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aider: lignes de commande et time-sheet mis à jour.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,25 +7,26 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.10-14" sheetId="12" r:id="rId1"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId2"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId3"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId4"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId5"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId6"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId7"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId8"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId9"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId10"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId11"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId12"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId1"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId2"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId3"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId4"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId5"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId6"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId7"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId8"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId9"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId10"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="134">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -418,6 +419,15 @@
   </si>
   <si>
     <t>Facturé le 29.03.2015</t>
+  </si>
+  <si>
+    <t>TODO, point 38</t>
+  </si>
+  <si>
+    <t>Analyse et e-mails</t>
+  </si>
+  <si>
+    <t>Production export Bonne Nouvelle</t>
   </si>
 </sst>
 </file>
@@ -831,7 +841,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,14 +891,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42065</v>
+        <v>42095</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="E4" s="2">
-        <v>5.5555555555555552E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G35" si="0">D4*F4</f>
@@ -900,16 +912,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42067</v>
+        <v>42113</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.3888888888888888E-2</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G9" si="1">D5*F5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -918,16 +931,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>42077</v>
+        <v>42116</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D6" s="2">
-        <v>5.5555555555555552E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -936,17 +949,17 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>42077</v>
+        <v>42117</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
-        <v>7.6388888888888895E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -954,17 +967,10 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>42081</v>
-      </c>
-      <c r="C8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -972,18 +978,10 @@
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>42082</v>
-      </c>
-      <c r="C9" t="s">
-        <v>128</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
       <c r="G9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -991,15 +989,8 @@
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>42092</v>
-      </c>
-      <c r="C10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1130,16 +1121,16 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>42065</v>
+        <v>42095</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D23" s="2">
-        <v>0.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G34" si="2">D23*F23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1147,17 +1138,10 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1">
-        <v>42066</v>
-      </c>
-      <c r="C24" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
       <c r="G24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1165,17 +1149,10 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
-        <v>42066</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="2">
-        <v>6.25E-2</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
       <c r="G25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1183,17 +1160,10 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <v>42067</v>
-      </c>
-      <c r="C26" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.125</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="G26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1201,17 +1171,10 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <v>42067</v>
-      </c>
-      <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.16666666666666666</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="G27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1219,17 +1182,10 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1">
-        <v>42069</v>
-      </c>
-      <c r="C28" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
       <c r="G28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1237,17 +1193,10 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1">
-        <v>42072</v>
-      </c>
-      <c r="C29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
       <c r="G29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1255,17 +1204,10 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1">
-        <v>42073</v>
-      </c>
-      <c r="C30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
       <c r="G30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1273,17 +1215,10 @@
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1">
-        <v>42075</v>
-      </c>
-      <c r="C31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1291,17 +1226,10 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="1">
-        <v>42076</v>
-      </c>
-      <c r="C32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1309,17 +1237,10 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1">
-        <v>42079</v>
-      </c>
-      <c r="C33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
       <c r="G33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1327,17 +1248,10 @@
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="1">
-        <v>42080</v>
-      </c>
-      <c r="C34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.20833333333333334</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
       <c r="G34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1345,15 +1259,8 @@
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="1">
-        <v>42081</v>
-      </c>
-      <c r="C35" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.25</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1362,11 +1269,11 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>2.5729166666666674</v>
+        <v>0.19791666666666666</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0.16666666666666669</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1386,11 +1293,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>2.5729166666666674</v>
+        <v>0.19791666666666666</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>61.75</v>
+        <v>4.75</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1402,7 +1309,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>9262.5</v>
+        <v>712.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1492,6 +1399,572 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>41778</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="G4" s="2">
+        <f>D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41779</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G28" si="0">D5*F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41780</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41782</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41782</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41785</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41792</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41795</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41796</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41760</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41761</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41764</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <f>D19*F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41768</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G20" s="2">
+        <f>D20*F20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41779</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8611111111111112E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41779</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41780</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11458333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41782</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41793</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.28125</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="13">
+        <f>SUM(D4:D30)</f>
+        <v>2.5138888888888888</v>
+      </c>
+      <c r="E31" s="13">
+        <f>SUM(E4:E30)</f>
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="13">
+        <f>SUM(G4:G30)</f>
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="13">
+        <f>SUM(I4:I30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="12">
+        <f>D31-G31</f>
+        <v>2.2152777777777777</v>
+      </c>
+      <c r="E33" s="10">
+        <f>INT(DAY(D33)*24+HOUR(D33))+MINUTE(D33)/60</f>
+        <v>53.166666666666664</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="10">
+        <f>E33*150</f>
+        <v>7975</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2057,18 +2530,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -2081,7 +2542,687 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42065</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42067</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G9" si="1">D5*F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42077</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42077</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42081</v>
+      </c>
+      <c r="C8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42082</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42092</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42065</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G34" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42066</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42066</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42067</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42067</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42069</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42072</v>
+      </c>
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42073</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42075</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42076</v>
+      </c>
+      <c r="C32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42079</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42080</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1">
+        <v>42081</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.5729166666666674</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>2.5729166666666674</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>61.75</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>9262.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2753,7 +3894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3348,7 +4489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3996,7 +5137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4614,7 +5755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5253,7 +6394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5915,7 +7056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6451,570 +7592,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>41778</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="7">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="G4" s="2">
-        <f>D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41779</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2">
-        <f t="shared" ref="G5:G28" si="0">D5*F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41780</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41782</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41782</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41785</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>41792</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41795</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>41796</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1">
-        <v>41760</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>41761</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1">
-        <v>41764</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G19" s="2">
-        <f>D19*F19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
-        <v>41768</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G20" s="2">
-        <f>D20*F20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>41779</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>4.8611111111111112E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>41779</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.23958333333333334</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41780</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11458333333333333</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>5.2083333333333336E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41782</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>41793</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.28125</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="13">
-        <f>SUM(D4:D30)</f>
-        <v>2.5138888888888888</v>
-      </c>
-      <c r="E31" s="13">
-        <f>SUM(E4:E30)</f>
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="13">
-        <f>SUM(G4:G30)</f>
-        <v>0.2986111111111111</v>
-      </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="13">
-        <f>SUM(I4:I30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="12">
-        <f>D31-G31</f>
-        <v>2.2152777777777777</v>
-      </c>
-      <c r="E33" s="10">
-        <f>INT(DAY(D33)*24+HOUR(D33))+MINUTE(D33)/60</f>
-        <v>53.166666666666664</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="10">
-        <f>E33*150</f>
-        <v>7975</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: mis à jour timesheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="135">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>Production export Bonne Nouvelle</t>
+  </si>
+  <si>
+    <t>Mise à jour, maintenance, etc.</t>
   </si>
 </sst>
 </file>
@@ -841,7 +844,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,8 +970,18 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="1">
+        <v>42126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1138,8 +1151,15 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="1">
+        <v>42121</v>
+      </c>
+      <c r="C24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3.125E-2</v>
+      </c>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1269,11 +1289,11 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.19791666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>4.8611111111111112E-2</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1293,11 +1313,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.19791666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>4.75</v>
+        <v>6</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1309,7 +1329,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>712.5</v>
+        <v>900</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Aider: mise à jour après pub. BN.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,26 +7,27 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId1"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId2"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId3"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId4"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId5"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId6"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId7"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId8"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId9"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId10"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId11"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId12"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId13"/>
+    <sheet name="2015.18-21" sheetId="14" r:id="rId1"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId2"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId3"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId4"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId5"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId6"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId7"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId8"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId9"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId10"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId11"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId13"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="139">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -431,6 +432,18 @@
   </si>
   <si>
     <t>Mise à jour, maintenance, etc.</t>
+  </si>
+  <si>
+    <t>Facturé le …</t>
+  </si>
+  <si>
+    <t>Corrections d'adresses + investigations</t>
+  </si>
+  <si>
+    <t>Fusion de Arzier-Le Muids</t>
+  </si>
+  <si>
+    <t>Exportation BN</t>
   </si>
 </sst>
 </file>
@@ -841,10 +854,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,17 +907,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42095</v>
+        <v>42130</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D4" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G35" si="0">D4*F4</f>
         <v>0</v>
@@ -915,14 +926,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42113</v>
+        <v>42139</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>2.0833333333333332E-2</v>
+        <v>137</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
@@ -934,13 +944,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>42116</v>
+        <v>42139</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2.0833333333333332E-2</v>
+        <v>138</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -951,16 +962,8 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>42117</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -970,18 +973,8 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>42126</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1134,13 +1127,13 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>42095</v>
+        <v>42139</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D23" s="2">
-        <v>0.16666666666666666</v>
+        <v>5.9027777777777783E-2</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
@@ -1151,15 +1144,8 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1">
-        <v>42121</v>
-      </c>
-      <c r="C24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="2">
-        <v>3.125E-2</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1289,11 +1275,11 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.25</v>
+        <v>0.12847222222222224</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>9.7222222222222224E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1313,11 +1299,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.25</v>
+        <v>0.12847222222222224</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>6</v>
+        <v>3.0833333333333335</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1329,7 +1315,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>900</v>
+        <v>462.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1409,6 +1395,17 @@
         <v>6262.5</v>
       </c>
       <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1419,6 +1416,544 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>41800</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <f>D4*F4</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41801</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G29" si="0">D5*F5</f>
+        <v>3.8194444444444441E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41807</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41809</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41815</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41816</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41817</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41819</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41821</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41800</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.15625</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41808</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41808</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="2">
+        <f>D20*F20</f>
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41808</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G21" s="2">
+        <f>D21*F21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41816</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41820</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="13">
+        <f>SUM(D4:D31)</f>
+        <v>1.1562499999999998</v>
+      </c>
+      <c r="E32" s="13">
+        <f>SUM(E4:E31)</f>
+        <v>4.8611111111111105E-2</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="13">
+        <f>SUM(G4:G31)</f>
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="I32" s="13">
+        <f>SUM(I4:I31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="12">
+        <f>D32-G32</f>
+        <v>0.84722222222222199</v>
+      </c>
+      <c r="E34" s="10">
+        <f>INT(DAY(D34)*24+HOUR(D34))+MINUTE(D34)/60</f>
+        <v>20.333333333333332</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="10">
+        <f>E34*150</f>
+        <v>3050</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1984,7 +2519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2550,18 +3085,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -2574,7 +3097,612 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42095</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42095</v>
+      </c>
+      <c r="C23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42121</v>
+      </c>
+      <c r="C24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>0.25</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>6</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>900</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3242,7 +4370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3914,7 +5042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4509,7 +5637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5157,7 +6285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5775,7 +6903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6414,7 +7542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7074,542 +8202,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>41800</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <f>D4*F4</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41801</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" ref="G5:G29" si="0">D5*F5</f>
-        <v>3.8194444444444441E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41807</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41809</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41815</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1388888888888889</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41816</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41817</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>41819</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41821</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>41800</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.15625</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1">
-        <v>41808</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
-        <v>41808</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="2">
-        <f>D20*F20</f>
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>41808</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G21" s="2">
-        <f>D21*F21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>41816</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41820</v>
-      </c>
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="13">
-        <f>SUM(D4:D31)</f>
-        <v>1.1562499999999998</v>
-      </c>
-      <c r="E32" s="13">
-        <f>SUM(E4:E31)</f>
-        <v>4.8611111111111105E-2</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="13">
-        <f>SUM(G4:G31)</f>
-        <v>0.30902777777777779</v>
-      </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="13">
-        <f>SUM(I4:I31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="12">
-        <f>D32-G32</f>
-        <v>0.84722222222222199</v>
-      </c>
-      <c r="E34" s="10">
-        <f>INT(DAY(D34)*24+HOUR(D34))+MINUTE(D34)/60</f>
-        <v>20.333333333333332</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="10">
-        <f>E34*150</f>
-        <v>3050</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
AIDER: supprimé exception rte du Jorat 1-43.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="143">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t>Investigations et maintenance</t>
+  </si>
+  <si>
+    <t>Rôles et cache</t>
+  </si>
+  <si>
+    <t>Titres</t>
+  </si>
+  <si>
+    <t>Route du Jorat</t>
   </si>
 </sst>
 </file>
@@ -860,7 +869,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,8 +995,15 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="1">
+        <v>42156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -997,8 +1013,15 @@
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="1">
+        <v>42157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1008,8 +1031,15 @@
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="1">
+        <v>42159</v>
+      </c>
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1175,8 +1205,15 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="1">
+        <v>42156</v>
+      </c>
+      <c r="C25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1295,7 +1332,7 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.31944444444444442</v>
+        <v>0.71875</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1319,11 +1356,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.31944444444444442</v>
+        <v>0.71875</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>7.666666666666667</v>
+        <v>17.25</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1335,7 +1372,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>1150</v>
+        <v>2587.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
AIDER: rend visible la colonne politesse.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="144">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>Route du Jorat</t>
+  </si>
+  <si>
+    <t>Adresses, politesse, etc.</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,8 +1052,15 @@
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="1">
+        <v>42161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1060,8 +1070,15 @@
       <c r="A12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="1">
+        <v>42164</v>
+      </c>
+      <c r="C12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1223,8 +1240,15 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="1">
+        <v>42159</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.27083333333333331</v>
+      </c>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1332,7 +1356,7 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.71875</v>
+        <v>1.0729166666666665</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1356,11 +1380,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.71875</v>
+        <v>1.0729166666666665</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>17.25</v>
+        <v>25.75</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1372,7 +1396,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>2587.5</v>
+        <v>3862.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Aider: lignes de commande et timesheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,28 +7,30 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.25-31" sheetId="15" r:id="rId1"/>
-    <sheet name="2015.18-24" sheetId="14" r:id="rId2"/>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId3"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId4"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId5"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId6"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId7"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId8"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId9"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId10"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId11"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId12"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId13"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId14"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId15"/>
+    <sheet name="2015.34-36" sheetId="17" r:id="rId1"/>
+    <sheet name="2015.31-33" sheetId="16" r:id="rId2"/>
+    <sheet name="2015.25-30" sheetId="15" r:id="rId3"/>
+    <sheet name="2015.18-24" sheetId="14" r:id="rId4"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId5"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId6"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId7"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId8"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId9"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId10"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId11"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId12"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId13"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId14"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId16"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId17"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="167">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -493,6 +495,42 @@
   </si>
   <si>
     <t>Divers, migrations, renommé municipalités</t>
+  </si>
+  <si>
+    <t>Facturé le 24.07.2015</t>
+  </si>
+  <si>
+    <t>Registres (Todo 114 et 117)</t>
+  </si>
+  <si>
+    <t>Qualité de données (Todo 109 et 111)</t>
+  </si>
+  <si>
+    <t>Registres (reporting)</t>
+  </si>
+  <si>
+    <t>Registres (validation)</t>
+  </si>
+  <si>
+    <t>Registres (tests, corrections)</t>
+  </si>
+  <si>
+    <t>Registres (améliorations)</t>
+  </si>
+  <si>
+    <t>Registres (tests, reporting)</t>
+  </si>
+  <si>
+    <t>Registres (tests, validation)</t>
+  </si>
+  <si>
+    <t>Registres et todo 78 et 79</t>
+  </si>
+  <si>
+    <t>Migration, importations RCH</t>
+  </si>
+  <si>
+    <t>Facturé le 17.08.2015</t>
   </si>
 </sst>
 </file>
@@ -575,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -598,6 +636,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -903,10 +943,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,16 +996,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42178</v>
+        <v>42233</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="D4" s="2">
-        <v>0.125</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <f t="shared" ref="G4:G37" si="0">D4*F4</f>
         <v>0</v>
       </c>
     </row>
@@ -974,12 +1014,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42179</v>
+        <v>42234</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D5" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E5" s="2">
         <v>9.7222222222222224E-2</v>
       </c>
       <c r="G5" s="2">
@@ -991,16 +1034,9 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>42180</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1010,18 +1046,9 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>42184</v>
-      </c>
-      <c r="C7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1031,16 +1058,9 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>42208</v>
-      </c>
-      <c r="C8" t="s">
-        <v>154</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>0.1388888888888889</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1050,15 +1070,8 @@
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>42208</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3.472222222222222E-3</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1199,15 +1212,8 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="1">
-        <v>42178</v>
-      </c>
-      <c r="C23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.20833333333333334</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="D23" s="2"/>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1217,15 +1223,8 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1">
-        <v>42184</v>
-      </c>
-      <c r="C24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.34375</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1235,15 +1234,8 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
-        <v>42185</v>
-      </c>
-      <c r="C25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1253,15 +1245,8 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <v>42186</v>
-      </c>
-      <c r="C26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1271,15 +1256,8 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <v>42191</v>
-      </c>
-      <c r="C27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.3125</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1289,15 +1267,8 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1">
-        <v>42192</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1307,15 +1278,8 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1">
-        <v>42207</v>
-      </c>
-      <c r="C29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1354,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1365,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1376,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1387,14 +1351,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>2.854166666666667</v>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0.24305555555555555</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1407,36 +1389,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>2.854166666666667</v>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>68.5</v>
+        <v>1.75</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>22</v>
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>10275</v>
+        <v>262.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>24</v>
       </c>
@@ -1447,7 +1429,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>43</v>
       </c>
@@ -1458,7 +1440,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>72</v>
       </c>
@@ -1469,7 +1451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>79</v>
       </c>
@@ -1480,7 +1462,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>91</v>
       </c>
@@ -1532,6 +1514,28 @@
         <v>4300</v>
       </c>
       <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1542,6 +1546,1263 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41918</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41919</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41922</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41929</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41936</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41941</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41942</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41917</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41918</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41918</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41918</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41919</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41925</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41942</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>0.9375</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>22.5</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>3375</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41898</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G5" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41904</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41905</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" ref="G6:G35" si="1">D6*F6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41911</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41912</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41898</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41899</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41900</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41901</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41904</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41905</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>41906</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>41907</v>
+      </c>
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1">
+        <v>41908</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>41911</v>
+      </c>
+      <c r="C33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1">
+        <v>41912</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>3.5833333333333339</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>1.9270833333333335</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.6562500000000004</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>39.75</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>5962.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2203,7 +3464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2741,7 +4002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3307,7 +4568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3873,7 +5134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3885,7 +5146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3898,6 +5159,1362 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C54" sqref="C54:F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42232</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G37" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42208</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42209</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42213</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42214</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42215</v>
+      </c>
+      <c r="C27" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42216</v>
+      </c>
+      <c r="C28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42220</v>
+      </c>
+      <c r="C29" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42221</v>
+      </c>
+      <c r="C30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42222</v>
+      </c>
+      <c r="C31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42223</v>
+      </c>
+      <c r="C32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42226</v>
+      </c>
+      <c r="C33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42227</v>
+      </c>
+      <c r="C34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1">
+        <v>42228</v>
+      </c>
+      <c r="C35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>42229</v>
+      </c>
+      <c r="C36" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>42230</v>
+      </c>
+      <c r="C37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>3.7187500000000004</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>3.7187500000000004</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>89.25</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>13387.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42178</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42208</v>
+      </c>
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42208</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42178</v>
+      </c>
+      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42184</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42185</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42186</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42191</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42192</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42207</v>
+      </c>
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.854166666666667</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>2.854166666666667</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>68.5</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>10275</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4562,7 +7179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5155,7 +7772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5823,7 +8440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6495,7 +9112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7090,7 +9707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7736,1261 +10353,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>41918</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41919</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41922</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41929</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41936</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41941</v>
-      </c>
-      <c r="C9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41942</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41917</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41918</v>
-      </c>
-      <c r="C24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41918</v>
-      </c>
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41918</v>
-      </c>
-      <c r="C26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41919</v>
-      </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>41925</v>
-      </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1">
-        <v>41942</v>
-      </c>
-      <c r="C29" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.21527777777777779</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>0.9375</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>0.9375</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>22.5</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>3375</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>41898</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G5" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41904</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41905</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" ref="G6:G35" si="1">D6*F6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41911</v>
-      </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41912</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="G23" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41898</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41899</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41900</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41901</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>41904</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="F28" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="1"/>
-        <v>0.15625</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1">
-        <v>41905</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F29" s="8">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1">
-        <v>41906</v>
-      </c>
-      <c r="C30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F30" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1">
-        <v>41907</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="F31" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1">
-        <v>41908</v>
-      </c>
-      <c r="C32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F32" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1">
-        <v>41911</v>
-      </c>
-      <c r="C33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F33" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1">
-        <v>41912</v>
-      </c>
-      <c r="C34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F34" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>3.5833333333333339</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>7.9861111111111105E-2</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>1.9270833333333335</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>1.6562500000000004</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>39.75</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>5962.5</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: met à jour les lignes de commandes et timesheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,30 +7,31 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.34-36" sheetId="17" r:id="rId1"/>
-    <sheet name="2015.31-33" sheetId="16" r:id="rId2"/>
-    <sheet name="2015.25-30" sheetId="15" r:id="rId3"/>
-    <sheet name="2015.18-24" sheetId="14" r:id="rId4"/>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId5"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId6"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId7"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId8"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId9"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId10"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId11"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId12"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId13"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId14"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId15"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId16"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId17"/>
+    <sheet name="2015.39-42" sheetId="18" r:id="rId1"/>
+    <sheet name="2015.34-38" sheetId="17" r:id="rId2"/>
+    <sheet name="2015.31-33" sheetId="16" r:id="rId3"/>
+    <sheet name="2015.25-30" sheetId="15" r:id="rId4"/>
+    <sheet name="2015.18-24" sheetId="14" r:id="rId5"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId6"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId7"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId8"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId9"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId10"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId11"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId12"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId13"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId14"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId15"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId16"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId17"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="176">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -531,6 +532,33 @@
   </si>
   <si>
     <t>Facturé le 17.08.2015</t>
+  </si>
+  <si>
+    <t>Correctif urgent - liste des gestions</t>
+  </si>
+  <si>
+    <t>Analyse et correctifs</t>
+  </si>
+  <si>
+    <t>Sortie des ménages</t>
+  </si>
+  <si>
+    <t>Mailings</t>
+  </si>
+  <si>
+    <t>Debug éditeur de requêtes</t>
+  </si>
+  <si>
+    <t>Éditeur de requêtes, refonte</t>
+  </si>
+  <si>
+    <t>Mises à jour</t>
+  </si>
+  <si>
+    <t>Adaptations diverses</t>
+  </si>
+  <si>
+    <t>Facturé le 18.09.2015</t>
   </si>
 </sst>
 </file>
@@ -943,10 +971,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B23" sqref="B23:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,13 +1024,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42233</v>
+        <v>42264</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D4" s="2">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G37" si="0">D4*F4</f>
@@ -1013,18 +1041,9 @@
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>42234</v>
-      </c>
-      <c r="C5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>9.7222222222222224E-2</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1372,11 +1391,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>7.2916666666666671E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>9.7222222222222224E-2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1396,11 +1415,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>7.2916666666666671E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>1.75</v>
+        <v>0.25</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1412,7 +1431,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>262.5</v>
+        <v>37.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1536,6 +1555,17 @@
         <v>13387.5</v>
       </c>
       <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1546,6 +1576,654 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41954</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G11" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41957</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41963</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41967</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41974</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>7.2916666666666671E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41975</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41977</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41984</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41988</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" ref="G12:G35" si="1">D12*F12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41947</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G31" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41949</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41954</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41956</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41962</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41968</v>
+      </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41969</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>41970</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>41975</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.020833333333333</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>9.722222222222221E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.864583333333333</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>44.75</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>6712.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2163,7 +2841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2802,7 +3480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3464,7 +4142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4002,7 +4680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4568,7 +5246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5134,18 +5812,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -5158,7 +5824,716 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G37" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42234</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42243</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42263</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42261</v>
+      </c>
+      <c r="C23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42262</v>
+      </c>
+      <c r="C24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42262</v>
+      </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42263</v>
+      </c>
+      <c r="C26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42263</v>
+      </c>
+      <c r="C27" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42264</v>
+      </c>
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42265</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>36</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>5400</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5860,7 +7235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6514,7 +7889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7179,7 +8554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7772,7 +9147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8440,7 +9815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9112,7 +10487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9705,652 +11080,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>41954</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G11" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41957</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41963</v>
-      </c>
-      <c r="C6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41967</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41974</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41975</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41977</v>
-      </c>
-      <c r="C10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>41984</v>
-      </c>
-      <c r="C11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41988</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" ref="G12:G35" si="1">D12*F12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41947</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="2">
-        <f t="shared" ref="G23:G31" si="2">D23*F23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41949</v>
-      </c>
-      <c r="C24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41954</v>
-      </c>
-      <c r="C25" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41956</v>
-      </c>
-      <c r="C26" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41962</v>
-      </c>
-      <c r="C27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>41968</v>
-      </c>
-      <c r="C28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1">
-        <v>41969</v>
-      </c>
-      <c r="C29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1">
-        <v>41970</v>
-      </c>
-      <c r="C30" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1">
-        <v>41975</v>
-      </c>
-      <c r="C31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>2.020833333333333</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>9.722222222222221E-2</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>1.864583333333333</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>44.75</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>6712.5</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: commandes et time-sheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,31 +7,32 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.39-42" sheetId="18" r:id="rId1"/>
-    <sheet name="2015.34-38" sheetId="17" r:id="rId2"/>
-    <sheet name="2015.31-33" sheetId="16" r:id="rId3"/>
-    <sheet name="2015.25-30" sheetId="15" r:id="rId4"/>
-    <sheet name="2015.18-24" sheetId="14" r:id="rId5"/>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId6"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId7"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId8"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId9"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId10"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId11"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId12"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId13"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId14"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId15"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId16"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId17"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId18"/>
+    <sheet name="2015.43-45" sheetId="19" r:id="rId1"/>
+    <sheet name="2015.39-42" sheetId="18" r:id="rId2"/>
+    <sheet name="2015.34-38" sheetId="17" r:id="rId3"/>
+    <sheet name="2015.31-33" sheetId="16" r:id="rId4"/>
+    <sheet name="2015.25-30" sheetId="15" r:id="rId5"/>
+    <sheet name="2015.18-24" sheetId="14" r:id="rId6"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId7"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId8"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId9"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId10"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId11"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId12"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId13"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId14"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId15"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId16"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId17"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId18"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId19"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="190">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -574,6 +575,33 @@
   </si>
   <si>
     <t>Job de nettoyage ECH</t>
+  </si>
+  <si>
+    <t>Divers, debug, etc.</t>
+  </si>
+  <si>
+    <t>Debug + TODO 105</t>
+  </si>
+  <si>
+    <t>Requêtes et mailings</t>
+  </si>
+  <si>
+    <t>Export CSV, partenaires A et B, warnings</t>
+  </si>
+  <si>
+    <t>Flux de traitement des warnings</t>
+  </si>
+  <si>
+    <t>Expérimentations</t>
+  </si>
+  <si>
+    <t>Dépannage urgent</t>
+  </si>
+  <si>
+    <t>Facturé le 19.10.2015</t>
+  </si>
+  <si>
+    <t>Mise à jour Renens, rue de la Gare</t>
   </si>
 </sst>
 </file>
@@ -986,10 +1014,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,13 +1067,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42264</v>
+        <v>42298</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
       <c r="D4" s="2">
-        <v>1.0416666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G37" si="0">D4*F4</f>
@@ -1056,16 +1087,9 @@
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>42269</v>
-      </c>
-      <c r="C5" t="s">
-        <v>179</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1075,15 +1099,8 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>42272</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1094,16 +1111,9 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>42276</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1267,15 +1277,8 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="1">
-        <v>42269</v>
-      </c>
-      <c r="C23" t="s">
-        <v>176</v>
-      </c>
-      <c r="D23" s="2">
-        <v>6.25E-2</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="D23" s="2"/>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1285,15 +1288,8 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1">
-        <v>42269</v>
-      </c>
-      <c r="C24" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.10416666666666667</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1303,15 +1299,8 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
-        <v>42269</v>
-      </c>
-      <c r="C25" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.125</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1321,15 +1310,8 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <v>42269</v>
-      </c>
-      <c r="C26" t="s">
-        <v>178</v>
-      </c>
-      <c r="D26" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1339,15 +1321,8 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <v>42270</v>
-      </c>
-      <c r="C27" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.29166666666666669</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1357,6 +1332,7 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
+      <c r="B28" s="1"/>
       <c r="D28" s="2"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
@@ -1378,15 +1354,8 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1">
-        <v>42276</v>
-      </c>
-      <c r="C30" t="s">
-        <v>176</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.3125</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1448,6 +1417,9 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
       <c r="B36" s="1"/>
       <c r="D36" s="2"/>
       <c r="G36" s="2">
@@ -1468,11 +1440,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.96180555555555558</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1492,11 +1464,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.96180555555555558</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>23.083333333333332</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1508,7 +1480,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>3462.5</v>
+        <v>50</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1643,6 +1615,17 @@
         <v>5400</v>
       </c>
       <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="9">
+        <v>10200</v>
+      </c>
+      <c r="F56" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1653,6 +1636,601 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42007</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42012</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42014</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42028</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42034</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" ref="G16:G29" si="1">D16*F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41982</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G26" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41983</v>
+      </c>
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41984</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41988</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41996</v>
+      </c>
+      <c r="C27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="2">
+        <f t="shared" ref="G30:G35" si="3">D30*F30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>1.1631944444444444</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.1180555555555556</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>26.833333333333332</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>4025</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2300,7 +2878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2918,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3557,7 +4135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4219,7 +4797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4757,7 +5335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5323,7 +5901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5889,18 +6467,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -5913,7 +6479,768 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42264</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G37" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42269</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42272</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42276</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42269</v>
+      </c>
+      <c r="C23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42269</v>
+      </c>
+      <c r="C24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42269</v>
+      </c>
+      <c r="C25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42269</v>
+      </c>
+      <c r="C26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42270</v>
+      </c>
+      <c r="C27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42271</v>
+      </c>
+      <c r="C28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42272</v>
+      </c>
+      <c r="C29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42276</v>
+      </c>
+      <c r="C30" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42277</v>
+      </c>
+      <c r="C31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42278</v>
+      </c>
+      <c r="C32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42283</v>
+      </c>
+      <c r="C33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42282</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1">
+        <v>42284</v>
+      </c>
+      <c r="C35" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1">
+        <v>42285</v>
+      </c>
+      <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.8368055555555549</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>2.8368055555555549</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>68.083333333333329</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>10212.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="9">
+        <v>10200</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6610,7 +7937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7312,7 +8639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7966,7 +9293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8631,7 +9958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9224,7 +10551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9892,7 +11219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -10562,599 +11889,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42007</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42012</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>42014</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42028</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>42034</v>
-      </c>
-      <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="2">
-        <v>4.5138888888888888E-2</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>4.5138888888888888E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" ref="G16:G29" si="1">D16*F16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41982</v>
-      </c>
-      <c r="C23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="2">
-        <f t="shared" ref="G23:G26" si="2">D23*F23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41983</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41984</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.25694444444444448</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41988</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41996</v>
-      </c>
-      <c r="C27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="2">
-        <f t="shared" ref="G30:G35" si="3">D30*F30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>1.1631944444444444</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>0.1875</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>4.5138888888888888E-2</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>1.1180555555555556</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>26.833333333333332</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>4025</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: adapte le téléchargement depuis ftp.vd.ch.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="2015.43-45" sheetId="19" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="205">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -602,6 +602,51 @@
   </si>
   <si>
     <t>Mise à jour Renens, rue de la Gare</t>
+  </si>
+  <si>
+    <t>Envoie BN, maintenance</t>
+  </si>
+  <si>
+    <t>Divers, e-mails</t>
+  </si>
+  <si>
+    <t>Préparation et analyse</t>
+  </si>
+  <si>
+    <t>Réflexion, modélisation des proc. de sortie</t>
+  </si>
+  <si>
+    <t>Processus de sortie des personnes</t>
+  </si>
+  <si>
+    <t>Tests et améliorations du proc. de sortie</t>
+  </si>
+  <si>
+    <t>Modif. Serveur FTP de vd.ch</t>
+  </si>
+  <si>
+    <t>Gestion MAT[CH]</t>
+  </si>
+  <si>
+    <t>Tests, diverses vérifications, mails</t>
+  </si>
+  <si>
+    <t>Corrections</t>
+  </si>
+  <si>
+    <t>Abonnements BN</t>
+  </si>
+  <si>
+    <t>Processus</t>
+  </si>
+  <si>
+    <t>Divers, support, recherches</t>
+  </si>
+  <si>
+    <t>Maintenance, divers</t>
+  </si>
+  <si>
+    <t>Export BN, suivi</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1062,7 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,9 +1132,16 @@
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>42299</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1099,8 +1151,15 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="1">
+        <v>42300</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1111,8 +1170,15 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="1">
+        <v>42303</v>
+      </c>
+      <c r="C7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
@@ -1123,8 +1189,15 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="1">
+        <v>42320</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
@@ -1135,8 +1208,15 @@
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="1">
+        <v>42320</v>
+      </c>
+      <c r="C9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1146,8 +1226,18 @@
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="1">
+        <v>42326</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1157,8 +1247,18 @@
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="1">
+        <v>42327</v>
+      </c>
+      <c r="C11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1277,8 +1377,15 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="1">
+        <v>42313</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1288,8 +1395,15 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="1">
+        <v>42314</v>
+      </c>
+      <c r="C24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1299,8 +1413,15 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="1">
+        <v>42317</v>
+      </c>
+      <c r="C25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1310,8 +1431,15 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="1">
+        <v>42318</v>
+      </c>
+      <c r="C26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1321,8 +1449,15 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="1">
+        <v>42319</v>
+      </c>
+      <c r="C27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1332,8 +1467,15 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="1">
+        <v>42320</v>
+      </c>
+      <c r="C28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1343,8 +1485,15 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
+      <c r="B29" s="1">
+        <v>42321</v>
+      </c>
+      <c r="C29" t="s">
+        <v>194</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.1875</v>
+      </c>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1354,8 +1503,15 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
+      <c r="B30" s="1">
+        <v>42324</v>
+      </c>
+      <c r="C30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1365,8 +1521,15 @@
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
+      <c r="B31" s="1">
+        <v>42325</v>
+      </c>
+      <c r="C31" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1376,8 +1539,15 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="1">
+        <v>42326</v>
+      </c>
+      <c r="C32" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1387,8 +1557,15 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
+      <c r="B33" s="1">
+        <v>42327</v>
+      </c>
+      <c r="C33" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1398,8 +1575,15 @@
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="1">
+        <v>42327</v>
+      </c>
+      <c r="C34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1440,11 +1624,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>1.3888888888888888E-2</v>
+        <v>2.25</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.2986111111111111</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1464,11 +1648,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>1.3888888888888888E-2</v>
+        <v>2.25</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>0.33333333333333331</v>
+        <v>54</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1480,7 +1664,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>50</v>
+        <v>8100</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
- Aider: affiche aussi les LogMessage en mode Release.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,34 +7,35 @@
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
-    <sheet name="2015.51-53" sheetId="21" r:id="rId1"/>
-    <sheet name="2015.48-50" sheetId="20" r:id="rId2"/>
-    <sheet name="2015.43-47" sheetId="19" r:id="rId3"/>
-    <sheet name="2015.39-42" sheetId="18" r:id="rId4"/>
-    <sheet name="2015.34-38" sheetId="17" r:id="rId5"/>
-    <sheet name="2015.31-33" sheetId="16" r:id="rId6"/>
-    <sheet name="2015.25-30" sheetId="15" r:id="rId7"/>
-    <sheet name="2015.18-24" sheetId="14" r:id="rId8"/>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId9"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId10"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId11"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId12"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId13"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId14"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId15"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId16"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId17"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId18"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId19"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId20"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId21"/>
+    <sheet name="2016.06-09" sheetId="22" r:id="rId1"/>
+    <sheet name="2015.51-53" sheetId="21" r:id="rId2"/>
+    <sheet name="2015.48-50" sheetId="20" r:id="rId3"/>
+    <sheet name="2015.43-47" sheetId="19" r:id="rId4"/>
+    <sheet name="2015.39-42" sheetId="18" r:id="rId5"/>
+    <sheet name="2015.34-38" sheetId="17" r:id="rId6"/>
+    <sheet name="2015.31-33" sheetId="16" r:id="rId7"/>
+    <sheet name="2015.25-30" sheetId="15" r:id="rId8"/>
+    <sheet name="2015.18-24" sheetId="14" r:id="rId9"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId10"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId11"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId12"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId13"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId14"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId15"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId16"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId17"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId18"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId19"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId20"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId21"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId22"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="234">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -721,6 +722,21 @@
   </si>
   <si>
     <t>Migration Krios, mise à jour AIDER</t>
+  </si>
+  <si>
+    <t>Correctifs divers</t>
+  </si>
+  <si>
+    <t>Suite des correctifs, dérogations</t>
+  </si>
+  <si>
+    <t>Investigations et dépannages</t>
+  </si>
+  <si>
+    <t>Investigations (Line Dépraz)</t>
+  </si>
+  <si>
+    <t>Dérogations et RCH</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1163,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,17 +1213,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42356</v>
+        <v>42407</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D4" s="22">
-        <v>0.14583333333333334</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="E4" s="21"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
+        <f t="shared" ref="G4:G9" si="0">D4*F4</f>
         <v>0</v>
       </c>
     </row>
@@ -1216,15 +1232,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42357</v>
+        <v>42408</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D5" s="22">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="E5" s="21"/>
+        <v>6</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1234,14 +1250,14 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="24">
-        <v>42401</v>
+      <c r="B6" s="1">
+        <v>42410</v>
       </c>
       <c r="C6" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="D6" s="22">
-        <v>2.7777777777777776E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="E6" s="21"/>
       <c r="G6" s="2">
@@ -1253,16 +1269,9 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>42402</v>
-      </c>
-      <c r="C7" t="s">
-        <v>228</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="22">
-        <v>7.2916666666666671E-2</v>
-      </c>
+      <c r="E7" s="21"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1300,7 +1309,7 @@
       <c r="D10" s="22"/>
       <c r="E10" s="21"/>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G10:G37" si="1">D10*F10</f>
         <v>0</v>
       </c>
     </row>
@@ -1312,7 +1321,7 @@
       <c r="D11" s="22"/>
       <c r="E11" s="21"/>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1324,7 +1333,7 @@
       <c r="D12" s="22"/>
       <c r="E12" s="21"/>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1336,7 +1345,7 @@
       <c r="D13" s="22"/>
       <c r="E13" s="21"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1348,7 +1357,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="21"/>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1360,7 +1369,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="21"/>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1372,7 +1381,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="21"/>
       <c r="G16" s="2">
-        <f t="shared" ref="G16:G37" si="1">D16*F16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1441,17 +1450,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>42352</v>
+        <v>42405</v>
       </c>
       <c r="C23" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D23" s="23">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E23" s="20"/>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G28" si="2">D23*F23</f>
+        <f t="shared" ref="G23:G29" si="2">D23*F23</f>
         <v>0</v>
       </c>
     </row>
@@ -1460,13 +1469,13 @@
         <v>13</v>
       </c>
       <c r="B24" s="1">
-        <v>42352</v>
+        <v>42408</v>
       </c>
       <c r="C24" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="D24" s="23">
-        <v>0.20833333333333334</v>
+        <v>3.125E-2</v>
       </c>
       <c r="E24" s="20"/>
       <c r="G24" s="2">
@@ -1479,13 +1488,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="1">
-        <v>42353</v>
+        <v>42412</v>
       </c>
       <c r="C25" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="D25" s="23">
-        <v>8.3333333333333329E-2</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="E25" s="20"/>
       <c r="G25" s="2">
@@ -1497,15 +1506,8 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <v>42356</v>
-      </c>
-      <c r="C26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D26" s="23">
-        <v>0.14583333333333334</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="G26" s="2">
         <f t="shared" si="2"/>
@@ -1516,15 +1518,8 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <v>42391</v>
-      </c>
-      <c r="C27" t="s">
-        <v>225</v>
-      </c>
-      <c r="D27" s="23">
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="G27" s="2">
         <f t="shared" si="2"/>
@@ -1535,15 +1530,8 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1">
-        <v>42396</v>
-      </c>
-      <c r="C28" t="s">
-        <v>226</v>
-      </c>
-      <c r="D28" s="23">
-        <v>0.1875</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="G28" s="2">
         <f t="shared" si="2"/>
@@ -1554,18 +1542,11 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1">
-        <v>42397</v>
-      </c>
-      <c r="C29" t="s">
-        <v>227</v>
-      </c>
-      <c r="D29" s="23">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="G29" s="2">
-        <f t="shared" ref="G29:G35" si="3">D29*F29</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1577,7 +1558,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="G30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1589,7 +1570,7 @@
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="G31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1601,7 +1582,7 @@
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="G32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1613,7 +1594,7 @@
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="G33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1625,7 +1606,7 @@
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="G34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1637,7 +1618,7 @@
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="G35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1667,11 +1648,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>1.2812500000000002</v>
+        <v>0.40972222222222221</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>7.2916666666666671E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1691,11 +1672,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>1.2812500000000002</v>
+        <v>0.40972222222222221</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>30.75</v>
+        <v>9.8333333333333339</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1707,7 +1688,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>4612.5</v>
+        <v>1475</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1885,6 +1866,599 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42095</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42095</v>
+      </c>
+      <c r="C23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42121</v>
+      </c>
+      <c r="C24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>0.25</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>6</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>900</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2552,7 +3126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3224,7 +3798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3819,7 +4393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4467,7 +5041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5085,7 +5659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5724,7 +6298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6386,7 +6960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6924,7 +7498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7490,7 +8064,752 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42356</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42357</v>
+      </c>
+      <c r="C5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="22">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="24">
+        <v>42401</v>
+      </c>
+      <c r="C6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="22">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42402</v>
+      </c>
+      <c r="C7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="21"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="G16" s="2">
+        <f t="shared" ref="G16:G37" si="1">D16*F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42352</v>
+      </c>
+      <c r="C23" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G28" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42352</v>
+      </c>
+      <c r="C24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42353</v>
+      </c>
+      <c r="C25" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42356</v>
+      </c>
+      <c r="C26" t="s">
+        <v>223</v>
+      </c>
+      <c r="D26" s="23">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42391</v>
+      </c>
+      <c r="C27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="23">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42396</v>
+      </c>
+      <c r="C28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0.1875</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42397</v>
+      </c>
+      <c r="C29" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="G29" s="2">
+        <f t="shared" ref="G29:G35" si="3">D29*F29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="G33" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="G34" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="G35" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="21"/>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>1.2812500000000002</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.2812500000000002</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>30.75</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>4612.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="9">
+        <v>10200</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>206</v>
+      </c>
+      <c r="E57" s="9">
+        <v>8700</v>
+      </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" s="9">
+        <v>9475</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8056,7 +9375,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8875,31 +10218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9671,7 +10990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -10420,7 +11739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11117,7 +12436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11819,7 +13138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12473,7 +13792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13136,597 +14455,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42095</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42113</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>42116</v>
-      </c>
-      <c r="C6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42117</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>42126</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>42095</v>
-      </c>
-      <c r="C23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>42121</v>
-      </c>
-      <c r="C24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>0.25</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>0.25</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>6</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>900</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="E49" s="9">
-        <v>4025</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>130</v>
-      </c>
-      <c r="E50" s="9">
-        <v>6262.5</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="9">
-        <v>900</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Common: corrige un (très) vieux bug de conversion HTML malformé (boucle infinie)
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="237">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -737,6 +737,15 @@
   </si>
   <si>
     <t>Dérogations et RCH</t>
+  </si>
+  <si>
+    <t>Panne, recherches</t>
+  </si>
+  <si>
+    <t>Data Quality #12</t>
+  </si>
+  <si>
+    <t>Erreur MAT[CH] pour Ph. Morel</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1172,7 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,9 +1278,18 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21"/>
+      <c r="B7" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E7" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1281,8 +1299,15 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="22"/>
+      <c r="B8" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="22">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E8" s="21"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
@@ -1506,8 +1531,15 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="20"/>
+      <c r="B26" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="23">
+        <v>5.2083333333333336E-2</v>
+      </c>
       <c r="E26" s="20"/>
       <c r="G26" s="2">
         <f t="shared" si="2"/>
@@ -1518,8 +1550,15 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="23">
+        <v>3.125E-2</v>
+      </c>
       <c r="E27" s="20"/>
       <c r="G27" s="2">
         <f t="shared" si="2"/>
@@ -1648,11 +1687,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.40972222222222221</v>
+        <v>0.52083333333333326</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>5.5555555555555552E-2</v>
+        <v>9.722222222222221E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1672,11 +1711,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.40972222222222221</v>
+        <v>0.52083333333333326</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>9.8333333333333339</v>
+        <v>12.5</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1688,7 +1727,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>1475</v>
+        <v>1875</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Aider: lignes de commandes et time sheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,35 +7,36 @@
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
-    <sheet name="2016.06-09" sheetId="22" r:id="rId1"/>
-    <sheet name="2015.51-53" sheetId="21" r:id="rId2"/>
-    <sheet name="2015.48-50" sheetId="20" r:id="rId3"/>
-    <sheet name="2015.43-47" sheetId="19" r:id="rId4"/>
-    <sheet name="2015.39-42" sheetId="18" r:id="rId5"/>
-    <sheet name="2015.34-38" sheetId="17" r:id="rId6"/>
-    <sheet name="2015.31-33" sheetId="16" r:id="rId7"/>
-    <sheet name="2015.25-30" sheetId="15" r:id="rId8"/>
-    <sheet name="2015.18-24" sheetId="14" r:id="rId9"/>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId10"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId11"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId12"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId13"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId14"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId15"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId16"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId17"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId18"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId19"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId20"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId21"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId22"/>
+    <sheet name="2016.10-15" sheetId="23" r:id="rId1"/>
+    <sheet name="2016.06-09" sheetId="22" r:id="rId2"/>
+    <sheet name="2015.51-53" sheetId="21" r:id="rId3"/>
+    <sheet name="2015.48-50" sheetId="20" r:id="rId4"/>
+    <sheet name="2015.43-47" sheetId="19" r:id="rId5"/>
+    <sheet name="2015.39-42" sheetId="18" r:id="rId6"/>
+    <sheet name="2015.34-38" sheetId="17" r:id="rId7"/>
+    <sheet name="2015.31-33" sheetId="16" r:id="rId8"/>
+    <sheet name="2015.25-30" sheetId="15" r:id="rId9"/>
+    <sheet name="2015.18-24" sheetId="14" r:id="rId10"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId11"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId12"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId13"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId14"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId15"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId16"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId17"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId18"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId19"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId20"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId21"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId22"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId23"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="248">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -746,6 +747,39 @@
   </si>
   <si>
     <t>Erreur MAT[CH] pour Ph. Morel</t>
+  </si>
+  <si>
+    <t>Recherches de problèmes</t>
+  </si>
+  <si>
+    <t>Correction pour les ménages</t>
+  </si>
+  <si>
+    <t>Facturé le 28.01.2016</t>
+  </si>
+  <si>
+    <t>Investigations bonne nouvelle</t>
+  </si>
+  <si>
+    <t>Facturé le 07.03.2016</t>
+  </si>
+  <si>
+    <t>Suivi GitLiab, correctifs, etc.</t>
+  </si>
+  <si>
+    <t>Mise à jour RCH</t>
+  </si>
+  <si>
+    <t>Mises à jour, BN, maintenance</t>
+  </si>
+  <si>
+    <t>Recherches, adaptations d'adresses</t>
+  </si>
+  <si>
+    <t>DataQuality 13, Reporting 6</t>
+  </si>
+  <si>
+    <t>Décès</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1203,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,17 +1256,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42407</v>
+        <v>42444</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D4" s="22">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E4" s="21"/>
+        <v>243</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22">
+        <v>9.375E-2</v>
+      </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G9" si="0">D4*F4</f>
+        <f t="shared" ref="G4:G37" si="0">D4*F4</f>
         <v>0</v>
       </c>
     </row>
@@ -1241,15 +1275,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42408</v>
+        <v>42446</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22">
-        <v>5.5555555555555552E-2</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E5" s="22"/>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1260,15 +1294,15 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>42410</v>
+        <v>42447</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D6" s="22">
+        <v>244</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="E6" s="21"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1279,16 +1313,14 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>42412</v>
+        <v>42454</v>
       </c>
       <c r="C7" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="22">
-        <v>1.3888888888888888E-2</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="D7" s="22"/>
       <c r="E7" s="22">
-        <v>4.1666666666666664E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
@@ -1300,13 +1332,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="1">
-        <v>42412</v>
+        <v>42454</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="D8" s="22">
-        <v>1.3888888888888888E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="E8" s="21"/>
       <c r="G8" s="2">
@@ -1332,9 +1364,9 @@
       </c>
       <c r="B10" s="1"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
+      <c r="E10" s="22"/>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G37" si="1">D10*F10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1346,7 +1378,7 @@
       <c r="D11" s="22"/>
       <c r="E11" s="21"/>
       <c r="G11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1358,7 +1390,7 @@
       <c r="D12" s="22"/>
       <c r="E12" s="21"/>
       <c r="G12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1370,7 +1402,7 @@
       <c r="D13" s="22"/>
       <c r="E13" s="21"/>
       <c r="G13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1382,7 +1414,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="21"/>
       <c r="G14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1394,7 +1426,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="21"/>
       <c r="G15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1406,7 +1438,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="21"/>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1418,7 +1450,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="21"/>
       <c r="G17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1430,7 +1462,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="21"/>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1439,7 +1471,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="21"/>
       <c r="G19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1448,7 +1480,7 @@
       <c r="D20" s="22"/>
       <c r="E20" s="21"/>
       <c r="G20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1457,7 +1489,7 @@
       <c r="D21" s="22"/>
       <c r="E21" s="21"/>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1466,7 +1498,7 @@
       <c r="D22" s="22"/>
       <c r="E22" s="21"/>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1475,17 +1507,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>42405</v>
+        <v>42440</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>115</v>
       </c>
       <c r="D23" s="23">
-        <v>0.16666666666666666</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E23" s="20"/>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G29" si="2">D23*F23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1494,17 +1526,17 @@
         <v>13</v>
       </c>
       <c r="B24" s="1">
-        <v>42408</v>
+        <v>42446</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="D24" s="23">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
       <c r="E24" s="20"/>
       <c r="G24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1513,17 +1545,17 @@
         <v>13</v>
       </c>
       <c r="B25" s="1">
-        <v>42412</v>
+        <v>42451</v>
       </c>
       <c r="C25" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="D25" s="23">
-        <v>0.10069444444444443</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="E25" s="20"/>
       <c r="G25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1532,17 +1564,17 @@
         <v>13</v>
       </c>
       <c r="B26" s="1">
-        <v>42412</v>
+        <v>42472</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>247</v>
       </c>
       <c r="D26" s="23">
-        <v>5.2083333333333336E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="E26" s="20"/>
       <c r="G26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1550,18 +1582,11 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <v>42412</v>
-      </c>
-      <c r="C27" t="s">
-        <v>235</v>
-      </c>
-      <c r="D27" s="23">
-        <v>3.125E-2</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="20"/>
       <c r="G27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1570,10 +1595,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="20"/>
       <c r="G28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1585,7 +1610,7 @@
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="G29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1597,7 +1622,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="G30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1609,7 +1634,7 @@
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="G31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1621,7 +1646,7 @@
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1633,7 +1658,7 @@
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="G33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1645,7 +1670,7 @@
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="G34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1657,7 +1682,7 @@
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="G35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1669,7 +1694,7 @@
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L36" s="18"/>
@@ -1679,7 +1704,7 @@
       <c r="D37" s="22"/>
       <c r="E37" s="21"/>
       <c r="G37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L37" s="19"/>
@@ -1687,11 +1712,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.52083333333333326</v>
+        <v>0.37847222222222221</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>9.722222222222221E-2</v>
+        <v>0.2048611111111111</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1711,11 +1736,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.52083333333333326</v>
+        <v>0.37847222222222221</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>12.5</v>
+        <v>9.0833333333333339</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1727,7 +1752,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>1875</v>
+        <v>1362.5</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1895,6 +1920,28 @@
         <v>9475</v>
       </c>
       <c r="F58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="9">
+        <v>4612.5</v>
+      </c>
+      <c r="F59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>241</v>
+      </c>
+      <c r="E60" s="9">
+        <v>2400</v>
+      </c>
+      <c r="F60" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1905,6 +1952,671 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42139</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42159</v>
+      </c>
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42164</v>
+      </c>
+      <c r="C12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42166</v>
+      </c>
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42167</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42156</v>
+      </c>
+      <c r="C25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42159</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42166</v>
+      </c>
+      <c r="C27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="2">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>1.1944444444444444</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.14583333333333331</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.1944444444444444</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>28.666666666666668</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>4300</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2497,7 +3209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3165,7 +3877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3837,7 +4549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4432,7 +5144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5080,7 +5792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5698,7 +6410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6337,7 +7049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6999,7 +7711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7537,7 +8249,797 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42407</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G9" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42408</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42410</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E7" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="22">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42422</v>
+      </c>
+      <c r="C9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42424</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" ref="G10:G37" si="1">D10*F10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42436</v>
+      </c>
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="22">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42405</v>
+      </c>
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" s="23">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G29" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42408</v>
+      </c>
+      <c r="C24" t="s">
+        <v>230</v>
+      </c>
+      <c r="D24" s="23">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="23">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="23">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="23">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42424</v>
+      </c>
+      <c r="C28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="23">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="21"/>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>16</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>2400</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="9">
+        <v>10200</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>206</v>
+      </c>
+      <c r="E57" s="9">
+        <v>8700</v>
+      </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" s="9">
+        <v>9475</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="9">
+        <v>4612.5</v>
+      </c>
+      <c r="F59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>241</v>
+      </c>
+      <c r="E60" s="9">
+        <v>2400</v>
+      </c>
+      <c r="F60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8103,752 +9605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:L58"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42356</v>
-      </c>
-      <c r="C4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D4" s="22">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="E4" s="21"/>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42357</v>
-      </c>
-      <c r="C5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D5" s="22">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="24">
-        <v>42401</v>
-      </c>
-      <c r="C6" t="s">
-        <v>227</v>
-      </c>
-      <c r="D6" s="22">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42402</v>
-      </c>
-      <c r="C7" t="s">
-        <v>228</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22">
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21"/>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="21"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="21"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="21"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="21"/>
-      <c r="G16" s="2">
-        <f t="shared" ref="G16:G37" si="1">D16*F16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="21"/>
-      <c r="G17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="21"/>
-      <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="21"/>
-      <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="21"/>
-      <c r="G20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="21"/>
-      <c r="G21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="21"/>
-      <c r="G22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>42352</v>
-      </c>
-      <c r="C23" t="s">
-        <v>220</v>
-      </c>
-      <c r="D23" s="23">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="G23" s="2">
-        <f t="shared" ref="G23:G28" si="2">D23*F23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>42352</v>
-      </c>
-      <c r="C24" t="s">
-        <v>221</v>
-      </c>
-      <c r="D24" s="23">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="G24" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>42353</v>
-      </c>
-      <c r="C25" t="s">
-        <v>222</v>
-      </c>
-      <c r="D25" s="23">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="G25" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>42356</v>
-      </c>
-      <c r="C26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D26" s="23">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="G26" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>42391</v>
-      </c>
-      <c r="C27" t="s">
-        <v>225</v>
-      </c>
-      <c r="D27" s="23">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="G27" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>42396</v>
-      </c>
-      <c r="C28" t="s">
-        <v>226</v>
-      </c>
-      <c r="D28" s="23">
-        <v>0.1875</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="G28" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1">
-        <v>42397</v>
-      </c>
-      <c r="C29" t="s">
-        <v>227</v>
-      </c>
-      <c r="D29" s="23">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="G29" s="2">
-        <f t="shared" ref="G29:G35" si="3">D29*F29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="G30" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="G31" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="G32" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="G33" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="G34" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="G35" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="18"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="21"/>
-      <c r="G37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="19"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>1.2812500000000002</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>7.2916666666666671E-2</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>1.2812500000000002</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>30.75</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>4612.5</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="E49" s="9">
-        <v>4025</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>130</v>
-      </c>
-      <c r="E50" s="9">
-        <v>6262.5</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="9">
-        <v>900</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="9">
-        <v>4300</v>
-      </c>
-      <c r="F52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>155</v>
-      </c>
-      <c r="E53" s="9">
-        <v>10275</v>
-      </c>
-      <c r="F53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>166</v>
-      </c>
-      <c r="E54" s="9">
-        <v>13387.5</v>
-      </c>
-      <c r="F54" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>175</v>
-      </c>
-      <c r="E55" s="9">
-        <v>5400</v>
-      </c>
-      <c r="F55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" s="9">
-        <v>10200</v>
-      </c>
-      <c r="F56" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>206</v>
-      </c>
-      <c r="E57" s="9">
-        <v>8700</v>
-      </c>
-      <c r="F57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>219</v>
-      </c>
-      <c r="E58" s="9">
-        <v>9475</v>
-      </c>
-      <c r="F58" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9414,18 +10171,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -9438,7 +10183,764 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42356</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G15" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42357</v>
+      </c>
+      <c r="C5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="22">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="24">
+        <v>42401</v>
+      </c>
+      <c r="C6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="22">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42402</v>
+      </c>
+      <c r="C7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="21"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="G16" s="2">
+        <f t="shared" ref="G16:G37" si="1">D16*F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42352</v>
+      </c>
+      <c r="C23" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="G23" s="2">
+        <f t="shared" ref="G23:G28" si="2">D23*F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42352</v>
+      </c>
+      <c r="C24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42353</v>
+      </c>
+      <c r="C25" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42356</v>
+      </c>
+      <c r="C26" t="s">
+        <v>223</v>
+      </c>
+      <c r="D26" s="23">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42391</v>
+      </c>
+      <c r="C27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="23">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42396</v>
+      </c>
+      <c r="C28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0.1875</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42397</v>
+      </c>
+      <c r="C29" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="G29" s="2">
+        <f t="shared" ref="G29:G35" si="3">D29*F29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="G33" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="G34" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="G35" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="21"/>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>1.2812500000000002</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>1.2812500000000002</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>30.75</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>4612.5</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="9">
+        <v>10200</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>206</v>
+      </c>
+      <c r="E57" s="9">
+        <v>8700</v>
+      </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" s="9">
+        <v>9475</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -10257,7 +11759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11029,7 +12531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11778,7 +13280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12475,7 +13977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13177,7 +14679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13829,669 +15331,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42130</v>
-      </c>
-      <c r="C4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42139</v>
-      </c>
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>42139</v>
-      </c>
-      <c r="C6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>42156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>42157</v>
-      </c>
-      <c r="C9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>42159</v>
-      </c>
-      <c r="C10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>42161</v>
-      </c>
-      <c r="C11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>42164</v>
-      </c>
-      <c r="C12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D12" s="2">
-        <v>6.9444444444444434E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>42166</v>
-      </c>
-      <c r="C13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1">
-        <v>42167</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>42139</v>
-      </c>
-      <c r="C23" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>42150</v>
-      </c>
-      <c r="C24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>42156</v>
-      </c>
-      <c r="C25" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>42159</v>
-      </c>
-      <c r="C26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>42166</v>
-      </c>
-      <c r="C27" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" s="2">
-        <v>6.5972222222222224E-2</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>1.1944444444444444</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>0.14583333333333331</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>1.1944444444444444</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>28.666666666666668</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>4300</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="E49" s="9">
-        <v>4025</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>130</v>
-      </c>
-      <c r="E50" s="9">
-        <v>6262.5</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="9">
-        <v>900</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="9">
-        <v>4300</v>
-      </c>
-      <c r="F52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: time-sheet à jour.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -7,36 +7,37 @@
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
-    <sheet name="2016.10-15" sheetId="23" r:id="rId1"/>
-    <sheet name="2016.06-09" sheetId="22" r:id="rId2"/>
-    <sheet name="2015.51-53" sheetId="21" r:id="rId3"/>
-    <sheet name="2015.48-50" sheetId="20" r:id="rId4"/>
-    <sheet name="2015.43-47" sheetId="19" r:id="rId5"/>
-    <sheet name="2015.39-42" sheetId="18" r:id="rId6"/>
-    <sheet name="2015.34-38" sheetId="17" r:id="rId7"/>
-    <sheet name="2015.31-33" sheetId="16" r:id="rId8"/>
-    <sheet name="2015.25-30" sheetId="15" r:id="rId9"/>
-    <sheet name="2015.18-24" sheetId="14" r:id="rId10"/>
-    <sheet name="2015.14-17" sheetId="13" r:id="rId11"/>
-    <sheet name="2015.10-13" sheetId="12" r:id="rId12"/>
-    <sheet name="2015.06-09" sheetId="11" r:id="rId13"/>
-    <sheet name="2015.01-05" sheetId="10" r:id="rId14"/>
-    <sheet name="2014.45-51" sheetId="9" r:id="rId15"/>
-    <sheet name="2014.40-44" sheetId="8" r:id="rId16"/>
-    <sheet name="2014.38-39" sheetId="7" r:id="rId17"/>
-    <sheet name="2014.33-37" sheetId="6" r:id="rId18"/>
-    <sheet name="2014.24-27" sheetId="5" r:id="rId19"/>
-    <sheet name="2014.21-23" sheetId="4" r:id="rId20"/>
-    <sheet name="2014.18-20" sheetId="1" r:id="rId21"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId22"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId23"/>
+    <sheet name="2016.21-30" sheetId="24" r:id="rId1"/>
+    <sheet name="2016.10-20" sheetId="23" r:id="rId2"/>
+    <sheet name="2016.06-09" sheetId="22" r:id="rId3"/>
+    <sheet name="2015.51-53" sheetId="21" r:id="rId4"/>
+    <sheet name="2015.48-50" sheetId="20" r:id="rId5"/>
+    <sheet name="2015.43-47" sheetId="19" r:id="rId6"/>
+    <sheet name="2015.39-42" sheetId="18" r:id="rId7"/>
+    <sheet name="2015.34-38" sheetId="17" r:id="rId8"/>
+    <sheet name="2015.31-33" sheetId="16" r:id="rId9"/>
+    <sheet name="2015.25-30" sheetId="15" r:id="rId10"/>
+    <sheet name="2015.18-24" sheetId="14" r:id="rId11"/>
+    <sheet name="2015.14-17" sheetId="13" r:id="rId12"/>
+    <sheet name="2015.10-13" sheetId="12" r:id="rId13"/>
+    <sheet name="2015.06-09" sheetId="11" r:id="rId14"/>
+    <sheet name="2015.01-05" sheetId="10" r:id="rId15"/>
+    <sheet name="2014.45-51" sheetId="9" r:id="rId16"/>
+    <sheet name="2014.40-44" sheetId="8" r:id="rId17"/>
+    <sheet name="2014.38-39" sheetId="7" r:id="rId18"/>
+    <sheet name="2014.33-37" sheetId="6" r:id="rId19"/>
+    <sheet name="2014.24-27" sheetId="5" r:id="rId20"/>
+    <sheet name="2014.21-23" sheetId="4" r:id="rId21"/>
+    <sheet name="2014.18-20" sheetId="1" r:id="rId22"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId23"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId24"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="258">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -780,6 +781,36 @@
   </si>
   <si>
     <t>Décès</t>
+  </si>
+  <si>
+    <t>Panne RCH (Vaud), gestion, divers</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>Recherche d'erreurs dans l'adressage (BE)</t>
+  </si>
+  <si>
+    <t>DataQuality, RCH</t>
+  </si>
+  <si>
+    <t>Gestion des jobs</t>
+  </si>
+  <si>
+    <t>BN, mises à jour RCH, etc.</t>
+  </si>
+  <si>
+    <t>Facturé le 23.05.2016</t>
+  </si>
+  <si>
+    <t>Déploiement</t>
+  </si>
+  <si>
+    <t>Suivis GitLab</t>
+  </si>
+  <si>
+    <t>Gestion de projet, suivi, maintenance</t>
   </si>
 </sst>
 </file>
@@ -1203,10 +1234,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,14 +1287,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>42444</v>
+        <v>42513</v>
       </c>
       <c r="C4" t="s">
         <v>243</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22">
-        <v>9.375E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G37" si="0">D4*F4</f>
@@ -1275,10 +1306,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>42446</v>
+        <v>42514</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="D5" s="22">
         <v>1.0416666666666666E-2</v>
@@ -1294,14 +1325,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>42447</v>
+        <v>42519</v>
       </c>
       <c r="C6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D6" s="22"/>
+        <v>257</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E6" s="22">
-        <v>5.5555555555555552E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1312,16 +1345,9 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>42454</v>
-      </c>
-      <c r="C7" t="s">
-        <v>243</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="22">
-        <v>5.5555555555555552E-2</v>
-      </c>
+      <c r="E7" s="22"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1331,15 +1357,8 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>42454</v>
-      </c>
-      <c r="C8" t="s">
-        <v>245</v>
-      </c>
-      <c r="D8" s="22">
-        <v>5.5555555555555552E-2</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="21"/>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
@@ -1376,7 +1395,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="21"/>
+      <c r="E11" s="22"/>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1400,7 +1419,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="22"/>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1507,13 +1526,13 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>42440</v>
+        <v>42514</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="D23" s="23">
-        <v>4.1666666666666664E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="E23" s="20"/>
       <c r="G23" s="2">
@@ -1526,13 +1545,13 @@
         <v>13</v>
       </c>
       <c r="B24" s="1">
-        <v>42446</v>
+        <v>42516</v>
       </c>
       <c r="C24" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="D24" s="23">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="E24" s="20"/>
       <c r="G24" s="2">
@@ -1544,15 +1563,8 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
-        <v>42451</v>
-      </c>
-      <c r="C25" t="s">
-        <v>246</v>
-      </c>
-      <c r="D25" s="23">
-        <v>0.11458333333333333</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="20"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
@@ -1563,15 +1575,8 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <v>42472</v>
-      </c>
-      <c r="C26" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" s="23">
-        <v>3.125E-2</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="20"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
@@ -1607,7 +1612,7 @@
         <v>13</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="20"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
@@ -1712,11 +1717,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.37847222222222221</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0.2048611111111111</v>
+        <v>6.9444444444444448E-2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1736,11 +1741,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.37847222222222221</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>9.0833333333333339</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1752,7 +1757,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>1362.5</v>
+        <v>1100</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>
@@ -1942,6 +1947,17 @@
         <v>2400</v>
       </c>
       <c r="F60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>254</v>
+      </c>
+      <c r="E61" s="9">
+        <v>3350</v>
+      </c>
+      <c r="F61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1952,6 +1968,660 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42178</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42208</v>
+      </c>
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42208</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42178</v>
+      </c>
+      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42184</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42185</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42186</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42191</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42192</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42207</v>
+      </c>
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>2.854166666666667</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>2.854166666666667</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>68.5</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>10275</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2616,7 +3286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3209,7 +3879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3877,7 +4547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4549,7 +5219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5144,7 +5814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5792,7 +6462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6410,7 +7080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7049,7 +7719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7711,7 +8381,816 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L60"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42444</v>
+      </c>
+      <c r="C4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22">
+        <v>9.375E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G37" si="0">D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42446</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42447</v>
+      </c>
+      <c r="C6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42454</v>
+      </c>
+      <c r="C7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42454</v>
+      </c>
+      <c r="C8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42477</v>
+      </c>
+      <c r="C9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0.125</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42478</v>
+      </c>
+      <c r="C10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42479</v>
+      </c>
+      <c r="C11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42507</v>
+      </c>
+      <c r="C12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12" s="22">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42508</v>
+      </c>
+      <c r="C13" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42440</v>
+      </c>
+      <c r="C23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42446</v>
+      </c>
+      <c r="C24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.125</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42451</v>
+      </c>
+      <c r="C25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" s="23">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42472</v>
+      </c>
+      <c r="C26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" s="23">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42474</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42502</v>
+      </c>
+      <c r="C28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42513</v>
+      </c>
+      <c r="C29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29" s="23">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="21"/>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="13">
+        <f>SUM(D4:D37)</f>
+        <v>0.93055555555555558</v>
+      </c>
+      <c r="E38" s="13">
+        <f>SUM(E4:E37)</f>
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13">
+        <f>SUM(G4:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13">
+        <f>SUM(I4:I37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="12">
+        <f>D38-G38</f>
+        <v>0.93055555555555558</v>
+      </c>
+      <c r="E40" s="10">
+        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
+        <v>22.333333333333332</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="10">
+        <f>E40*150</f>
+        <v>3350</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7975.05</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4762.5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="9">
+        <v>5960</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="9">
+        <v>3375</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="9">
+        <v>4025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="9">
+        <v>6262.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="9">
+        <v>900</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="9">
+        <v>4300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="9">
+        <v>10275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="9">
+        <v>13387.5</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="9">
+        <v>5400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="9">
+        <v>10200</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>206</v>
+      </c>
+      <c r="E57" s="9">
+        <v>8700</v>
+      </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" s="9">
+        <v>9475</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="9">
+        <v>4612.5</v>
+      </c>
+      <c r="F59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>241</v>
+      </c>
+      <c r="E60" s="9">
+        <v>2400</v>
+      </c>
+      <c r="F60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8249,7 +9728,1163 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>41778</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="G4" s="2">
+        <f>D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41779</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G28" si="0">D5*F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41780</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41782</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41782</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41785</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41792</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41795</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41796</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41760</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41761</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41764</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <f>D19*F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41768</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G20" s="2">
+        <f>D20*F20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41779</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8611111111111112E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41779</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41780</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11458333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41781</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41782</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41793</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.28125</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="13">
+        <f>SUM(D4:D30)</f>
+        <v>2.5138888888888888</v>
+      </c>
+      <c r="E31" s="13">
+        <f>SUM(E4:E30)</f>
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="13">
+        <f>SUM(G4:G30)</f>
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="13">
+        <f>SUM(I4:I30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="12">
+        <f>D31-G31</f>
+        <v>2.2152777777777777</v>
+      </c>
+      <c r="E33" s="10">
+        <f>INT(DAY(D33)*24+HOUR(D33))+MINUTE(D33)/60</f>
+        <v>53.166666666666664</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="10">
+        <f>E33*150</f>
+        <v>7975</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>41767</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f>D4*F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41768</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G27" si="0">D5*F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41771</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41771</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41772</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41773</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41774</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41775</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41775</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41778</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41758</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41760</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2">
+        <f>I16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41761</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2">
+        <f>I17*F17</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41764</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="2">
+        <f>I18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41765</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41766</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41767</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41768</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2">
+        <f>I22*F22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41771</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41772</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41773</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41774</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41775</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="13">
+        <f>SUM(D4:D29)</f>
+        <v>2.3958333333333335</v>
+      </c>
+      <c r="E30" s="13">
+        <f>SUM(E4:E29)</f>
+        <v>0.33680555555555552</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="13">
+        <f>SUM(G4:G29)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="13">
+        <f>SUM(I4:I29)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="12">
+        <f>D30-G30</f>
+        <v>1.8958333333333335</v>
+      </c>
+      <c r="E32" s="10">
+        <f>INT(DAY(D32)*24+HOUR(D32))+MINUTE(D32)/60</f>
+        <v>45.5</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="10">
+        <f>E32*150</f>
+        <v>6825</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="9">
+        <v>6900</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9039,1163 +11674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>41778</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="7">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="G4" s="2">
-        <f>D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41779</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2">
-        <f t="shared" ref="G5:G28" si="0">D5*F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41780</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41782</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41782</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41785</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>41792</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41795</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>41796</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1">
-        <v>41760</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>41761</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1">
-        <v>41764</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G19" s="2">
-        <f>D19*F19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
-        <v>41768</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G20" s="2">
-        <f>D20*F20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>41779</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>4.8611111111111112E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>41779</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.23958333333333334</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41780</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11458333333333333</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>5.2083333333333336E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41781</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41782</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>41793</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.28125</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="13">
-        <f>SUM(D4:D30)</f>
-        <v>2.5138888888888888</v>
-      </c>
-      <c r="E31" s="13">
-        <f>SUM(E4:E30)</f>
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="13">
-        <f>SUM(G4:G30)</f>
-        <v>0.2986111111111111</v>
-      </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="13">
-        <f>SUM(I4:I30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="12">
-        <f>D31-G31</f>
-        <v>2.2152777777777777</v>
-      </c>
-      <c r="E33" s="10">
-        <f>INT(DAY(D33)*24+HOUR(D33))+MINUTE(D33)/60</f>
-        <v>53.166666666666664</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="10">
-        <f>E33*150</f>
-        <v>7975</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>41767</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E4" s="7">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G4" s="2">
-        <f>D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41768</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" ref="G5:G27" si="0">D5*F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>41771</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>41771</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41772</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.18055555555555555</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>41773</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>41774</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>41775</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>41775</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>41778</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>41758</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1">
-        <v>41760</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="2">
-        <f>I16*F16</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1">
-        <v>41761</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="2">
-        <f>I17*F17</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>41764</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="2">
-        <f>I18*F18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1">
-        <v>41765</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.18055555555555555</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
-        <v>41766</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>41767</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>41768</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="2">
-        <f>I22*F22</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41771</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41772</v>
-      </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41773</v>
-      </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41774</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41775</v>
-      </c>
-      <c r="C27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="13">
-        <f>SUM(D4:D29)</f>
-        <v>2.3958333333333335</v>
-      </c>
-      <c r="E30" s="13">
-        <f>SUM(E4:E29)</f>
-        <v>0.33680555555555552</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="13">
-        <f>SUM(G4:G29)</f>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="13">
-        <f>SUM(I4:I29)</f>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="12">
-        <f>D30-G30</f>
-        <v>1.8958333333333335</v>
-      </c>
-      <c r="E32" s="10">
-        <f>INT(DAY(D32)*24+HOUR(D32))+MINUTE(D32)/60</f>
-        <v>45.5</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="10">
-        <f>E32*150</f>
-        <v>6825</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -10940,7 +12419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11759,7 +13238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12531,7 +14010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13280,7 +14759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -13977,7 +15456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -14677,658 +16156,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:I53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42178</v>
-      </c>
-      <c r="C4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G35" si="0">D4*F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>42179</v>
-      </c>
-      <c r="C5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="2">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>42180</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42184</v>
-      </c>
-      <c r="C7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>42208</v>
-      </c>
-      <c r="C8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>42208</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="1">
-        <v>42178</v>
-      </c>
-      <c r="C23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>42184</v>
-      </c>
-      <c r="C24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.34375</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1">
-        <v>42185</v>
-      </c>
-      <c r="C25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>42186</v>
-      </c>
-      <c r="C26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>42191</v>
-      </c>
-      <c r="C27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1">
-        <v>42192</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1">
-        <v>42207</v>
-      </c>
-      <c r="C29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="13">
-        <f>SUM(D4:D37)</f>
-        <v>2.854166666666667</v>
-      </c>
-      <c r="E38" s="13">
-        <f>SUM(E4:E37)</f>
-        <v>0.24305555555555555</v>
-      </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="13">
-        <f>SUM(G4:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="13">
-        <f>SUM(I4:I37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="12">
-        <f>D38-G38</f>
-        <v>2.854166666666667</v>
-      </c>
-      <c r="E40" s="10">
-        <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>68.5</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="10">
-        <f>E40*150</f>
-        <v>10275</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="9">
-        <v>6900</v>
-      </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="9">
-        <v>7975.05</v>
-      </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="9">
-        <v>4762.5</v>
-      </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="9">
-        <v>5960</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="9">
-        <v>3375</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="E49" s="9">
-        <v>4025</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>130</v>
-      </c>
-      <c r="E50" s="9">
-        <v>6262.5</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="9">
-        <v>900</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="9">
-        <v>4300</v>
-      </c>
-      <c r="F52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>155</v>
-      </c>
-      <c r="E53" s="9">
-        <v>10275</v>
-      </c>
-      <c r="F53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Aider: lignes de commande, time-sheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="261">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -811,6 +811,15 @@
   </si>
   <si>
     <t>Gestion de projet, suivi, maintenance</t>
+  </si>
+  <si>
+    <t>Divers, suivi</t>
+  </si>
+  <si>
+    <t>Issue DQ/#3</t>
+  </si>
+  <si>
+    <t>Data Quality</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1246,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,8 +1354,15 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="D7" s="22"/>
+      <c r="B7" s="1">
+        <v>42523</v>
+      </c>
+      <c r="C7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="22">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="E7" s="22"/>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
@@ -1357,9 +1373,18 @@
       <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="1">
+        <v>42528</v>
+      </c>
+      <c r="C8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E8" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1563,8 +1588,15 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="23"/>
+      <c r="B25" s="1">
+        <v>42520</v>
+      </c>
+      <c r="C25" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E25" s="20"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
@@ -1575,8 +1607,15 @@
       <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="D26" s="23"/>
+      <c r="B26" s="1">
+        <v>42521</v>
+      </c>
+      <c r="C26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D26" s="23">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="E26" s="20"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
@@ -1587,8 +1626,15 @@
       <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="D27" s="23"/>
+      <c r="B27" s="1">
+        <v>42528</v>
+      </c>
+      <c r="C27" t="s">
+        <v>259</v>
+      </c>
+      <c r="D27" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E27" s="20"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
@@ -1717,11 +1763,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.30555555555555558</v>
+        <v>0.68749999999999989</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>6.9444444444444448E-2</v>
+        <v>0.125</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1741,11 +1787,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.30555555555555558</v>
+        <v>0.68749999999999989</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>7.333333333333333</v>
+        <v>16.5</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1757,7 +1803,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>1100</v>
+        <v>2475</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Aider: changement de nom de paroisse; Villeneuve - Haut-Lac.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="262">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -820,6 +820,9 @@
   </si>
   <si>
     <t>Data Quality</t>
+  </si>
+  <si>
+    <t>Villeneuve + divers</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1249,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,8 +1397,15 @@
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="D9" s="22"/>
+      <c r="B9" s="1">
+        <v>42535</v>
+      </c>
+      <c r="C9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="22">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="E9" s="21"/>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -1406,9 +1416,16 @@
       <c r="A10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>42536</v>
+      </c>
+      <c r="C10" t="s">
+        <v>243</v>
+      </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="E10" s="22">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1763,11 +1780,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.68749999999999989</v>
+        <v>0.73611111111111105</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>0.125</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1787,11 +1804,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.68749999999999989</v>
+        <v>0.73611111111111105</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>16.5</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1803,7 +1820,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>2475</v>
+        <v>2650</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
- Aider: corrige crash dans GetBestStreetName().
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="265">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -823,6 +823,15 @@
   </si>
   <si>
     <t>Villeneuve + divers</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>Suivi de projet</t>
+  </si>
+  <si>
+    <t>Bootstrap AIDER</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1258,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,8 +1444,15 @@
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="22"/>
+      <c r="B11" s="1">
+        <v>42551</v>
+      </c>
+      <c r="C11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E11" s="22"/>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -1447,8 +1463,15 @@
       <c r="A12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="1">
+        <v>42555</v>
+      </c>
+      <c r="C12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="22">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="E12" s="21"/>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
@@ -1662,8 +1685,15 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="D28" s="23"/>
+      <c r="B28" s="1">
+        <v>42551</v>
+      </c>
+      <c r="C28" t="s">
+        <v>262</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0.125</v>
+      </c>
       <c r="E28" s="20"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
@@ -1674,8 +1704,15 @@
       <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="D29" s="23"/>
+      <c r="B29" s="1">
+        <v>42555</v>
+      </c>
+      <c r="C29" t="s">
+        <v>264</v>
+      </c>
+      <c r="D29" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E29" s="20"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
@@ -1780,7 +1817,7 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>0.73611111111111105</v>
+        <v>0.90277777777777779</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
@@ -1804,11 +1841,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>0.73611111111111105</v>
+        <v>0.90277777777777779</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>17.666666666666668</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1820,7 +1857,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>2650</v>
+        <v>3250</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Aider: mise à jour lignes de commande et time sheet.
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
+++ b/Epsitec.Cresus/External/Documentation/Products/EERV - Aider/Time-sheet.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="274">
   <si>
     <t>Relevé des heures</t>
   </si>
@@ -851,6 +851,15 @@
   </si>
   <si>
     <t>Tentative de mise à jour MAT[CH]</t>
+  </si>
+  <si>
+    <t>Mise à jour de MAT[CH]</t>
+  </si>
+  <si>
+    <t>Recherches de solutions</t>
+  </si>
+  <si>
+    <t>Maintenance, nettoyage, etc.</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1286,7 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,8 +1373,15 @@
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="D6" s="22"/>
+      <c r="B6" s="1">
+        <v>42652</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="22">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="E6" s="21"/>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1376,9 +1392,16 @@
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>42676</v>
+      </c>
+      <c r="C7" t="s">
+        <v>273</v>
+      </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="21"/>
+      <c r="E7" s="22">
+        <v>0.125</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1575,8 +1598,15 @@
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="D24" s="20"/>
+      <c r="B24" s="1">
+        <v>42660</v>
+      </c>
+      <c r="C24" t="s">
+        <v>272</v>
+      </c>
+      <c r="D24" s="23">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="E24" s="20"/>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
@@ -1741,11 +1771,11 @@
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13">
         <f>SUM(D4:D37)</f>
-        <v>6.25E-2</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="E38" s="13">
         <f>SUM(E4:E37)</f>
-        <v>6.9444444444444434E-2</v>
+        <v>0.19444444444444442</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="13">
@@ -1765,11 +1795,11 @@
       </c>
       <c r="D40" s="12">
         <f>D38-G38</f>
-        <v>6.25E-2</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="E40" s="10">
         <f>INT(DAY(D40)*24+HOUR(D40))+MINUTE(D40)/60</f>
-        <v>1.5</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>25</v>
@@ -1781,7 +1811,7 @@
       </c>
       <c r="E41" s="10">
         <f>E40*150</f>
-        <v>225</v>
+        <v>1000</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>26</v>

</xml_diff>